<commit_message>
[IMP] Purged old unused code
</commit_message>
<xml_diff>
--- a/wok_code/tests/data/odoo_template_tnl.xlsx
+++ b/wok_code/tests/data/odoo_template_tnl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t xml:space="preserve">module</t>
   </si>
@@ -31,31 +31,175 @@
     <t xml:space="preserve">msgstr</t>
   </si>
   <si>
+    <t xml:space="preserve">test_module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;gt; 100%%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># invoice lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N. righe fattura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%s invoice lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">righe %s fattura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Invoice&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Fattura&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptance Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conto RI.BA. all'incasso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access to the Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accesso alla Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account.tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dear ${name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gentile ${name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome di battesimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fattura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Righe fattura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice n.%(number)s of %(date)s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fattura n.%(number)s di %(date)s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice n.%s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fattura n.%s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fattura/e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">riga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">righe </t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome di battesimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cognome</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name s.r.l.</t>
   </si>
   <si>
     <t xml:space="preserve">Nome s.r.l.</t>
   </si>
   <si>
-    <t xml:space="preserve">account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conto</t>
+    <t xml:space="preserve">Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print &lt;b&gt;Invoice&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stampa &lt;b&gt;Fattura&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquisto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Righe vendita</t>
   </si>
   <si>
     <t xml:space="preserve">tax</t>
@@ -68,132 +212,6 @@
   </si>
   <si>
     <t xml:space="preserve">EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fattura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;Invoice&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;Fattura&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print &lt;b&gt;Invoice&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stampa &lt;b&gt;Fattura&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice n.%s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fattura n.%s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice n.%(number)s of %(date)s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fattura n.%(number)s di %(date)s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fattura/e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">riga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">righe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Righe fattura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">account.tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gentile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear ${name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gentile ${name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acquisto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;gt; 100%%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%s invoice lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">righe %s fattura</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># invoice lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N. righe fattura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceptance Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conto RI.BA. all'incasso</t>
   </si>
 </sst>
 </file>
@@ -203,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +242,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,6 +303,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,10 +433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,72 +457,75 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -501,103 +533,103 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>44</v>
@@ -616,20 +648,20 @@
         <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>51</v>
@@ -657,6 +689,30 @@
       </c>
       <c r="C30" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>